<commit_message>
Finalizando Tema, falta apenas concluir a segunda regra bônus que não sei se vai dar tempo de fazer
</commit_message>
<xml_diff>
--- a/Lista de Classes.xlsx
+++ b/Lista de Classes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Guerreiros</t>
   </si>
@@ -496,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,27 +583,27 @@
         <v>18</v>
       </c>
       <c r="D4" s="2">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="P4" t="s">
         <v>33</v>
@@ -620,27 +620,27 @@
         <v>20</v>
       </c>
       <c r="D5" s="2">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="P5" t="s">
         <v>3</v>
@@ -657,27 +657,27 @@
         <v>21</v>
       </c>
       <c r="D6" s="2">
-        <v>800</v>
+        <v>300</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2">
-        <v>800</v>
+        <v>300</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="P6" t="s">
         <v>29</v>
@@ -701,17 +701,17 @@
         <v>30</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="2">
-        <v>300</v>
-      </c>
+      <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="2">
-        <v>300</v>
-      </c>
+      <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="L7" s="2">
+        <v>800</v>
+      </c>
       <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
+      <c r="N7" s="2">
+        <v>800</v>
+      </c>
       <c r="P7" t="s">
         <v>6</v>
       </c>
@@ -737,21 +737,17 @@
         <v>30</v>
       </c>
       <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
-        <v>30</v>
+      <c r="H8" s="2">
+        <v>800</v>
       </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
-        <v>30</v>
+      <c r="J8" s="2">
+        <v>800</v>
       </c>
       <c r="K8" s="2"/>
-      <c r="L8" s="2">
-        <v>500</v>
-      </c>
+      <c r="L8" s="2"/>
       <c r="M8" s="2"/>
-      <c r="N8" s="2">
-        <v>500</v>
-      </c>
+      <c r="N8" s="2"/>
       <c r="P8" t="s">
         <v>8</v>
       </c>
@@ -821,11 +817,11 @@
         <v>23</v>
       </c>
       <c r="D13" s="2">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2">
-        <v>50</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="3:20" x14ac:dyDescent="0.25">
@@ -897,11 +893,11 @@
         <v>28</v>
       </c>
       <c r="D23" s="2">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2">
-        <v>100</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>